<commit_message>
close to internal review
fixed missing figures
</commit_message>
<xml_diff>
--- a/doc/tables/VRML_management_history.xlsx
+++ b/doc/tables/VRML_management_history.xlsx
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -617,32 +617,32 @@
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10">
-        <v>15.957828368000003</v>
-      </c>
-      <c r="C4" s="10">
-        <v>19.19076055</v>
-      </c>
-      <c r="D4" s="10">
-        <v>14.854865627000001</v>
-      </c>
-      <c r="E4" s="10">
-        <v>11.128733288000001</v>
-      </c>
-      <c r="F4" s="10">
-        <v>14.520705443999999</v>
-      </c>
-      <c r="G4" s="10">
-        <v>12.774068973</v>
-      </c>
-      <c r="H4" s="10">
-        <v>21.284937983000003</v>
-      </c>
-      <c r="I4" s="10">
-        <v>23.612898744999999</v>
-      </c>
-      <c r="J4" s="10">
-        <v>26.891223343</v>
+      <c r="B4">
+        <v>15.249187881000001</v>
+      </c>
+      <c r="C4">
+        <v>18.694921457</v>
+      </c>
+      <c r="D4">
+        <v>14.149005886000001</v>
+      </c>
+      <c r="E4">
+        <v>10.504073128000002</v>
+      </c>
+      <c r="F4">
+        <v>13.471785277999999</v>
+      </c>
+      <c r="G4">
+        <v>12.103826680000001</v>
+      </c>
+      <c r="H4">
+        <v>20.602144877000001</v>
+      </c>
+      <c r="I4">
+        <v>22.948637797</v>
+      </c>
+      <c r="J4">
+        <v>25.695856503000002</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -653,31 +653,31 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>4.2208766730000002</v>
+        <v>4.2092349420000001</v>
       </c>
       <c r="C5">
-        <v>4.8845030339999997</v>
+        <v>4.8672359539999999</v>
       </c>
       <c r="D5">
-        <v>2.6750009179999998</v>
+        <v>2.6569098059999998</v>
       </c>
       <c r="E5">
-        <v>2.9707335719999999</v>
+        <v>2.9496996360000001</v>
       </c>
       <c r="F5">
-        <v>5.0663585649999998</v>
+        <v>5.0175686429999997</v>
       </c>
       <c r="G5">
-        <v>4.5897512130000004</v>
+        <v>4.5489877779999999</v>
       </c>
       <c r="H5">
-        <v>6.5573322190000001</v>
+        <v>6.4900402110000002</v>
       </c>
       <c r="I5">
-        <v>7.7476158799999997</v>
+        <v>7.630987287</v>
       </c>
       <c r="J5">
-        <v>7.9633027949999997</v>
+        <v>7.8841050680000002</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -688,31 +688,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>6.5099953040000003</v>
+        <v>6.101510019</v>
       </c>
       <c r="C6">
-        <v>9.4302280649999997</v>
+        <v>9.1498084370000008</v>
       </c>
       <c r="D6">
-        <v>6.642596502</v>
+        <v>6.3047681310000003</v>
       </c>
       <c r="E6">
-        <v>4.2995934370000004</v>
+        <v>3.9485168939999999</v>
       </c>
       <c r="F6">
-        <v>5.3150448389999996</v>
+        <v>4.6526362670000001</v>
       </c>
       <c r="G6">
-        <v>4.005105125</v>
+        <v>3.6893570389999999</v>
       </c>
       <c r="H6">
-        <v>9.0758563980000009</v>
+        <v>8.7976447980000003</v>
       </c>
       <c r="I6">
-        <v>9.4776576630000005</v>
+        <v>9.1994460629999999</v>
       </c>
       <c r="J6">
-        <v>10.042918278</v>
+        <v>9.2524440489999993</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -723,31 +723,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>1.2044755410000001</v>
+        <v>1.0010529029999999</v>
       </c>
       <c r="C7">
-        <v>1.0625501230000001</v>
+        <v>0.91056403900000005</v>
       </c>
       <c r="D7">
-        <v>1.5385199409999999</v>
+        <v>1.2793095059999999</v>
       </c>
       <c r="E7">
-        <v>1.195916038</v>
+        <v>0.95995894400000004</v>
       </c>
       <c r="F7">
-        <v>1.327752885</v>
+        <v>1.1406763470000001</v>
       </c>
       <c r="G7">
-        <v>1.23695311</v>
+        <v>0.99728770099999997</v>
       </c>
       <c r="H7">
-        <v>0.92312060399999996</v>
+        <v>0.73130381</v>
       </c>
       <c r="I7">
-        <v>1.2969511380000001</v>
+        <v>1.1505956959999999</v>
       </c>
       <c r="J7">
-        <v>2.764097558</v>
+        <v>2.496598257</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -758,31 +758,31 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>4.0204808500000002</v>
+        <v>3.935390017</v>
       </c>
       <c r="C8">
-        <v>3.8134793280000001</v>
+        <v>3.7673130270000001</v>
       </c>
       <c r="D8">
-        <v>3.996548266</v>
+        <v>3.9058184429999998</v>
       </c>
       <c r="E8">
-        <v>2.6604902410000002</v>
+        <v>2.6438976540000003</v>
       </c>
       <c r="F8">
-        <v>2.8115491549999998</v>
+        <v>2.6609040209999999</v>
       </c>
       <c r="G8">
-        <v>2.873209525</v>
+        <v>2.7991441620000002</v>
       </c>
       <c r="H8">
-        <v>4.7025005350000004</v>
+        <v>4.5570278310000001</v>
       </c>
       <c r="I8">
-        <v>5.0889286299999998</v>
+        <v>4.9658633170000002</v>
       </c>
       <c r="J8">
-        <v>6.1209047120000006</v>
+        <v>6.0627091290000008</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -904,31 +904,31 @@
         <v>6</v>
       </c>
       <c r="B12" s="10">
-        <v>212.05490463300001</v>
+        <v>210.31004203399996</v>
       </c>
       <c r="C12" s="10">
-        <v>237.477427742</v>
+        <v>235.21579864099999</v>
       </c>
       <c r="D12" s="10">
-        <v>239.11339173300001</v>
+        <v>237.074402177</v>
       </c>
       <c r="E12" s="10">
-        <v>198.74349890000002</v>
+        <v>197.04260851699999</v>
       </c>
       <c r="F12" s="10">
-        <v>337.03655141499996</v>
+        <v>334.98417319199996</v>
       </c>
       <c r="G12" s="10">
-        <v>293.36100764700001</v>
+        <v>292.37527859700003</v>
       </c>
       <c r="H12" s="10">
-        <v>342.35702047299998</v>
+        <v>341.20708119999995</v>
       </c>
       <c r="I12" s="10">
-        <v>346.100347548</v>
+        <v>344.453927615</v>
       </c>
       <c r="J12" s="10">
-        <v>489.25079224199999</v>
+        <v>484.96701131999998</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -936,31 +936,31 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>193.07020080000001</v>
+        <v>191.43732836199999</v>
       </c>
       <c r="C13">
-        <v>218.72607653</v>
+        <v>216.479694747</v>
       </c>
       <c r="D13">
-        <v>210.219318668</v>
+        <v>208.19767995699999</v>
       </c>
       <c r="E13">
-        <v>169.25350654600001</v>
+        <v>167.57198866100001</v>
       </c>
       <c r="F13">
-        <v>293.786203817</v>
+        <v>291.77875828399999</v>
       </c>
       <c r="G13">
-        <v>261.08552665299999</v>
+        <v>260.16175313100001</v>
       </c>
       <c r="H13">
-        <v>288.636152568</v>
+        <v>287.49309342599997</v>
       </c>
       <c r="I13">
-        <v>279.75047140700002</v>
+        <v>278.157520347</v>
       </c>
       <c r="J13">
-        <v>418.14599949199999</v>
+        <v>413.946043062</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -968,31 +968,31 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>17.040236423000003</v>
+        <v>16.928246262000002</v>
       </c>
       <c r="C14">
-        <v>16.657241212000002</v>
+        <v>16.641993894000002</v>
       </c>
       <c r="D14">
-        <v>26.618683066999999</v>
+        <v>26.601332221999996</v>
       </c>
       <c r="E14">
-        <v>26.626498356000003</v>
+        <v>26.607125858</v>
       </c>
       <c r="F14">
-        <v>39.714420600999993</v>
+        <v>39.669487910999997</v>
       </c>
       <c r="G14">
-        <v>29.210373999000002</v>
+        <v>29.148418471000003</v>
       </c>
       <c r="H14">
-        <v>48.201525496000002</v>
+        <v>48.194645365</v>
       </c>
       <c r="I14">
-        <v>59.697518007000006</v>
+        <v>59.644049134000007</v>
       </c>
       <c r="J14">
-        <v>67.272862754000002</v>
+        <v>67.189038262000011</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">

</xml_diff>